<commit_message>
Modificaciones a solicitud gráfica CN_10_11
Modificaciones a solicitud gráfica CN_10_11
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion11/SolicitudGrafica CN_10_11_CO.xlsx
+++ b/fuentes/contenidos/grado10/guion11/SolicitudGrafica CN_10_11_CO.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="hX79YNGfHMUCcosWMoH0GQuhNo2gkebFrfW3do2TOcvwqaujU9m0uwOL5UkRtWEspAy/ISD2JB8+jf057W9mVA==" workbookSaltValue="uRz/CDpmZ5ecKheoN1C0Jw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Solicitud gráfica" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="212">
   <si>
     <t>Fecha:</t>
   </si>
@@ -590,18 +590,18 @@
     <t>Trabajar un video</t>
   </si>
   <si>
-    <t xml:space="preserve">El enlace químico y la nomenclatura de compuestos inorgánicos </t>
+    <t>El enlace químico y la nomenclatura de compuestos inorgánicos</t>
   </si>
   <si>
     <t>Lyz Marcela Bernal Gómez</t>
   </si>
   <si>
+    <t>CN_10_11_CO</t>
+  </si>
+  <si>
     <t>Cuaderno de Estudio</t>
   </si>
   <si>
-    <t>CN_10_11_CO</t>
-  </si>
-  <si>
     <t>Código shutterstock 110129690</t>
   </si>
   <si>
@@ -611,12 +611,12 @@
     <t>Realizar ilustración igual a la imagen guía. Los colores de las letras, flecha y rectángulo se deja a consideración.</t>
   </si>
   <si>
+    <t>4° ESO/Física y Química/La estructura de la materia/Los enlaces químicos/Los esquemas de Lewis                            FQ_10_10_img4_small.jpg</t>
+  </si>
+  <si>
     <t>Fotografía</t>
   </si>
   <si>
-    <t>4° ESO/Física y Química/La estructura de la materia/Los enlaces químicos/Los esquemas de Lewis                            FQ_10_10_img4_small.jpg</t>
-  </si>
-  <si>
     <t>FQ_10_10_img4_small.jpg</t>
   </si>
   <si>
@@ -632,7 +632,7 @@
     <t>FQ_10_10_img2_small.jpg</t>
   </si>
   <si>
-    <t>Realizar ilustración igual a la imagen guía. LA imagen se tomo de 4° ESO/Física y Química/La estructura de la materia/Los enlaces químicos/enlace covalente                         FQ_10_10_img3_small.jpg</t>
+    <t xml:space="preserve">Realizar ilustración igual a la imagen guía. La imagen se tomo de 4° ESO/Física y Química/La estructura de la materia/Los enlaces químicos/enlace covalente       </t>
   </si>
   <si>
     <t>Realizar ilustración igual a la imagen guía. Se deja a consideración los colores. Manejar la letras Delta como se trabajaron en lMG05</t>
@@ -641,25 +641,16 @@
     <t xml:space="preserve">Realizar ilustración igual a la imagen guía. Se deja a criterio los colores </t>
   </si>
   <si>
-    <t>Realizar ilustración igual a la imagen guía. Por favor las esferas de color azul manejarlas de color blnco</t>
+    <t>Realizar ilustración igual a la imagen guía. Por favor las esferas de color azul manejarlas de color blanco</t>
   </si>
   <si>
     <t>Realizar ilustración igual a imagen guía. Por favor las esferas verde (-) realizarla de color rojo y las esferas de color rojo (+) realizarlas de color blanco. Por favor las esferas que estan en rojo pegarlas a la verde</t>
   </si>
   <si>
-    <t>Realizar ilustración igual a la imagen guía.Se deja a consideración el manejo de colores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tabla </t>
-  </si>
-  <si>
-    <t>Se comparte en Drive https://drive.google.com/file/d/0B8KYPZlXH19OWmx2R09uUkhyX0E/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>Realizar ilustración igual a imagen guía. Por favor los punto negros poner en el lado opuesto a como se encuentra en la imagen guía.La imagen no tiene pie de imagen porque va inmersa en la tabla IMG11</t>
-  </si>
-  <si>
-    <t>Realizar ilustración igual a imagen guía.La imagen no tiene pie de imagen porque va inmersa en la tabla IMG11</t>
+    <t>Tabla</t>
+  </si>
+  <si>
+    <t>Se comparte enlace https://drive.google.com/file/d/0B8KYPZlXH19ORlRHcXFBX00xT2M/view?usp=sharing</t>
   </si>
   <si>
     <t>Realizar ilustración igual a la imagen guía.</t>
@@ -1837,15 +1828,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
+      <xdr:colOff>182563</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
+      <xdr:rowOff>111124</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>3515360</xdr:colOff>
+      <xdr:colOff>2643188</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>1943099</xdr:rowOff>
+      <xdr:rowOff>1397000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1853,7 +1844,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1865,8 +1856,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="13830300" y="2200274"/>
-          <a:ext cx="3391535" cy="1876425"/>
+          <a:off x="13898563" y="2230437"/>
+          <a:ext cx="2460625" cy="1285876"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1875,8 +1866,8 @@
           <a:noFill/>
         </a:ln>
         <a:extLst>
-          <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
-            <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+          <a:ext uri="{53640926-AAD7-44d8-BBD7-CCE9431645EC}">
+            <a14:shadowObscured xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:w15="http://schemas.microsoft.com/office/word/2012/wordml" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns="" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas"/>
           </a:ext>
         </a:extLst>
       </xdr:spPr>
@@ -1886,15 +1877,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>790574</xdr:colOff>
+      <xdr:colOff>420687</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>222250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>2938779</xdr:colOff>
+      <xdr:colOff>2124392</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>1583055</xdr:rowOff>
+      <xdr:rowOff>1143000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1916,8 +1907,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="14497049" y="4562475"/>
-          <a:ext cx="2148205" cy="1478280"/>
+          <a:off x="14136687" y="3905250"/>
+          <a:ext cx="1703705" cy="920750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1935,15 +1926,254 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>1724025</xdr:colOff>
+          <xdr:colOff>684213</xdr:colOff>
           <xdr:row>11</xdr:row>
-          <xdr:rowOff>9710</xdr:rowOff>
+          <xdr:rowOff>41275</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>2676525</xdr:colOff>
+          <xdr:colOff>1638301</xdr:colOff>
           <xdr:row>11</xdr:row>
-          <xdr:rowOff>2238375</xdr:rowOff>
+          <xdr:rowOff>1344084</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2051" name="Object 3" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2051"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>264583</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>2080048</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1904365</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4" descr="http://profesores.aulaplaneta.com/DNNPlayerPackages/Package14355/InfoGuion/cuadernoestudio/images_xml/FQ_10_10_img2_zoom.jpg"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="13970000" y="6572250"/>
+          <a:ext cx="1815465" cy="1872615"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>84667</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>2208212</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1689630</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="14022917" y="8667750"/>
+          <a:ext cx="1890712" cy="1604963"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>105833</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>105834</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>3249083</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1686984</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 6"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:srcRect l="37944" t="37131" r="29648" b="38663"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="13811250" y="10625667"/>
+          <a:ext cx="3143250" cy="1581150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
+            <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>370416</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>381000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>3220773</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>3417146</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagen 7"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:srcRect l="33096" t="23546" r="33130" b="13967"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="14075833" y="12647083"/>
+          <a:ext cx="2850357" cy="3050699"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
+            <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>9</xdr:col>
+          <xdr:colOff>216695</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>407194</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>9</xdr:col>
+          <xdr:colOff>4012407</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>2700338</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1981,368 +2211,27 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>371474</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>2186939</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>1939289</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Imagen 4" descr="http://profesores.aulaplaneta.com/DNNPlayerPackages/Package14355/InfoGuion/cuadernoestudio/images_xml/FQ_10_10_img2_zoom.jpg"/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="14077949" y="8572499"/>
-          <a:ext cx="1815465" cy="1872615"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>428625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>3600450</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>2009775</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Imagen 8"/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:srcRect l="37944" t="37131" r="29648" b="38663"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="14163675" y="13220700"/>
-          <a:ext cx="3143250" cy="1581150"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
-            <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1028700</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>392908</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>2919412</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>1997871</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Imagen 11"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="14744700" y="11022808"/>
-          <a:ext cx="1890712" cy="1604963"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>428623</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>2214563</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>3278980</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>2943543</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Imagen 12"/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
-        <a:srcRect l="33096" t="23546" r="33130" b="13967"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="14120811" y="15025688"/>
-          <a:ext cx="2850357" cy="3050699"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
-            <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>130969</xdr:colOff>
-          <xdr:row>16</xdr:row>
-          <xdr:rowOff>226218</xdr:rowOff>
+          <xdr:colOff>200025</xdr:colOff>
+          <xdr:row>17</xdr:row>
+          <xdr:rowOff>57150</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>3940968</xdr:colOff>
-          <xdr:row>16</xdr:row>
-          <xdr:rowOff>2559843</xdr:rowOff>
+          <xdr:colOff>3876675</xdr:colOff>
+          <xdr:row>17</xdr:row>
+          <xdr:rowOff>2085975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="2062" name="Object 14" hidden="1">
+            <xdr:cNvPr id="2053" name="Object 5" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2062"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>9</xdr:col>
-          <xdr:colOff>202406</xdr:colOff>
-          <xdr:row>17</xdr:row>
-          <xdr:rowOff>523875</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>9</xdr:col>
-          <xdr:colOff>3881437</xdr:colOff>
-          <xdr:row>17</xdr:row>
-          <xdr:rowOff>2552700</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2063" name="Object 15" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2063"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>9</xdr:col>
-          <xdr:colOff>559594</xdr:colOff>
-          <xdr:row>18</xdr:row>
-          <xdr:rowOff>273843</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>9</xdr:col>
-          <xdr:colOff>3769519</xdr:colOff>
-          <xdr:row>18</xdr:row>
-          <xdr:rowOff>2340768</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2064" name="Object 16" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2064"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>9</xdr:col>
-          <xdr:colOff>321468</xdr:colOff>
-          <xdr:row>20</xdr:row>
-          <xdr:rowOff>392906</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>9</xdr:col>
-          <xdr:colOff>2007393</xdr:colOff>
-          <xdr:row>20</xdr:row>
-          <xdr:rowOff>1202531</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2066" name="Object 18" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2066"/>
+                  <a14:compatExt spid="_x0000_s2053"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2376,30 +2265,30 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>226219</xdr:rowOff>
+      <xdr:colOff>654843</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>2345531</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>1083469</xdr:rowOff>
+      <xdr:colOff>3833812</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>2455704</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Imagen 17"/>
+        <xdr:cNvPr id="11" name="Imagen 10"/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
-        <a:srcRect l="47352" t="66110" r="42804" b="25136"/>
+        <a:srcRect t="17862" r="61506" b="36368"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="14311313" y="30706219"/>
-          <a:ext cx="1726406" cy="857250"/>
+          <a:off x="14347031" y="22574250"/>
+          <a:ext cx="3178969" cy="2431892"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2419,30 +2308,30 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1012032</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>273844</xdr:rowOff>
+      <xdr:colOff>214313</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>2926557</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>2268379</xdr:rowOff>
+      <xdr:colOff>4214812</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>2381250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="Imagen 18"/>
+        <xdr:cNvPr id="12" name="Imagen 11"/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
-        <a:srcRect l="28513" t="23243" r="55363" b="46872"/>
+        <a:srcRect l="28512" t="24452" r="28208" b="44455"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="14704220" y="32004000"/>
-          <a:ext cx="1914525" cy="1994535"/>
+          <a:off x="13906501" y="25253156"/>
+          <a:ext cx="4000499" cy="2333625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2462,30 +2351,124 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>130969</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>261938</xdr:rowOff>
+      <xdr:colOff>511970</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>3631406</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>2967673</xdr:rowOff>
+      <xdr:colOff>3107532</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>2119313</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="Imagen 19"/>
+        <xdr:cNvPr id="13" name="Imagen 12" descr="Gastric Acid"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="14204158" y="28051126"/>
+          <a:ext cx="2595562" cy="2000250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>642937</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>178594</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>2720022</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>2075974</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Imagen 13" descr="Borax compounds for goldsmith specialist in gold"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="14335125" y="30265688"/>
+          <a:ext cx="2077085" cy="1897380"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>166688</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>4190999</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>2083593</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Imagen 14"/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
-        <a:srcRect t="17862" r="61506" b="36368"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:srcRect l="37338" t="41055" r="29397" b="42946"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="13823157" y="34480501"/>
-          <a:ext cx="3500437" cy="2705735"/>
+          <a:off x="13858876" y="32539781"/>
+          <a:ext cx="4024311" cy="1893093"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2505,210 +2488,30 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>261938</xdr:colOff>
+      <xdr:colOff>130970</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>178594</xdr:rowOff>
+      <xdr:rowOff>154782</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>5143499</xdr:colOff>
+      <xdr:colOff>4179094</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>2928938</xdr:rowOff>
+      <xdr:rowOff>1678782</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="Imagen 20"/>
+        <xdr:cNvPr id="16" name="Imagen 15"/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
-        <a:srcRect l="28512" t="24452" r="28208" b="44455"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="13954126" y="37861875"/>
-          <a:ext cx="4881561" cy="2750344"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
-            <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>559593</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>238125</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>3607592</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>2845594</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="22" name="Imagen 21" descr="Gastric Acid"/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="14251781" y="41338500"/>
-          <a:ext cx="3047999" cy="2607469"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>642937</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>678656</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>2720022</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>2576036</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="Imagen 22" descr="Borax compounds for goldsmith specialist in gold"/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="14335125" y="45100875"/>
-          <a:ext cx="2077085" cy="1897380"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>35719</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>5000625</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>1928812</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="24" name="Imagen 23"/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
-        <a:srcRect l="37338" t="41055" r="29397" b="42946"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="14025563" y="47458313"/>
-          <a:ext cx="4667250" cy="1893093"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
-            <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>273842</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>273844</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>5167311</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>1797844</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="25" name="Imagen 24"/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
         <a:srcRect l="36999" t="50111" r="28887" b="32079"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="13966030" y="50673000"/>
-          <a:ext cx="4893469" cy="1524000"/>
+          <a:off x="13823158" y="34635282"/>
+          <a:ext cx="4048124" cy="1524000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3443,9 +3246,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J31" sqref="J31"/>
+      <selection pane="bottomLeft" activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -3459,8 +3262,8 @@
     <col min="7" max="7" width="20.5" style="2" customWidth="1"/>
     <col min="8" max="8" width="28.625" style="2" customWidth="1"/>
     <col min="9" max="9" width="20.5" style="2" customWidth="1"/>
-    <col min="10" max="10" width="68.75" style="15" customWidth="1"/>
-    <col min="11" max="11" width="37" style="15" customWidth="1"/>
+    <col min="10" max="10" width="58.5" style="15" customWidth="1"/>
+    <col min="11" max="11" width="29.625" style="15" customWidth="1"/>
     <col min="12" max="12" width="20.375" style="2" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="14.5" style="2" hidden="1" customWidth="1"/>
     <col min="14" max="15" width="10.875" style="2" hidden="1" customWidth="1"/>
@@ -3560,7 +3363,7 @@
         <v>55</v>
       </c>
       <c r="G4" s="61" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H4" s="58"/>
       <c r="I4" s="38"/>
@@ -3639,7 +3442,7 @@
         <v>40</v>
       </c>
       <c r="C7" s="74" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>39</v>
@@ -3729,7 +3532,7 @@
         <v>M10B</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="11" customFormat="1" ht="183" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="11" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),"IMG01","")</f>
         <v>IMG01</v>
@@ -3772,20 +3575,20 @@
         <v>M12D</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="11" customFormat="1" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" s="11" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="str">
         <f t="shared" ref="A11:A18" si="3">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE(LEFT(A10,3),IF(MID(A10,4,2)+1&lt;10,CONCATENATE("0",MID(A10,4,2)+1))),"")</f>
         <v>IMG02</v>
       </c>
       <c r="B11" s="62" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C11" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D11" s="63" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E11" s="63" t="s">
         <v>154</v>
@@ -3815,7 +3618,7 @@
         <v>M101</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="11" customFormat="1" ht="179.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" s="11" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG03</v>
@@ -3849,7 +3652,7 @@
         <f ca="1">IF(OR($B12&lt;&gt;"",$J12&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E12,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E12,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J12"/>
+      <c r="J12" s="64"/>
       <c r="K12" s="64" t="s">
         <v>198</v>
       </c>
@@ -3858,7 +3661,7 @@
         <v>Diaporama F1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="11" customFormat="1" ht="163.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" s="11" customFormat="1" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG04</v>
@@ -3871,7 +3674,7 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D13" s="63" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E13" s="63" t="s">
         <v>154</v>
@@ -3901,7 +3704,7 @@
         <v>F4</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="11" customFormat="1" ht="174" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" s="11" customFormat="1" ht="152.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG05</v>
@@ -3944,7 +3747,7 @@
         <v>F6</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="11" customFormat="1" ht="183" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="11" customFormat="1" ht="137.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG06</v>
@@ -3978,7 +3781,7 @@
         <f ca="1">IF(OR($B15&lt;&gt;"",$J15&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E15,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E15,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J15"/>
+      <c r="J15" s="66"/>
       <c r="K15" s="66" t="s">
         <v>202</v>
       </c>
@@ -3987,7 +3790,7 @@
         <v>F6B</v>
       </c>
     </row>
-    <row r="16" spans="1:16" s="11" customFormat="1" ht="248.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" s="11" customFormat="1" ht="273" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG07</v>
@@ -4064,7 +3867,7 @@
         <f ca="1">IF(OR($B17&lt;&gt;"",$J17&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E17,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E17,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J17"/>
+      <c r="J17" s="66"/>
       <c r="K17" s="66" t="s">
         <v>204</v>
       </c>
@@ -4073,7 +3876,7 @@
         <v>F7B</v>
       </c>
     </row>
-    <row r="18" spans="1:15" s="11" customFormat="1" ht="273" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" s="11" customFormat="1" ht="211.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG09</v>
@@ -4107,7 +3910,7 @@
         <f ca="1">IF(OR($B18&lt;&gt;"",$J18&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E18,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E18,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J18"/>
+      <c r="J18" s="66"/>
       <c r="K18" s="66" t="s">
         <v>205</v>
       </c>
@@ -4116,7 +3919,7 @@
         <v>F8</v>
       </c>
     </row>
-    <row r="19" spans="1:15" s="11" customFormat="1" ht="252" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" s="11" customFormat="1" ht="57" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="str">
         <f t="shared" ref="A19:A50" si="6">IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),CONCATENATE(LEFT(A18,3),IF(MID(A18,4,2)+1&lt;10,CONCATENATE("0",MID(A18,4,2)+1),MID(A18,4,2)+1)),"")</f>
         <v>IMG10</v>
@@ -4150,16 +3953,18 @@
         <f ca="1">IF(OR($B19&lt;&gt;"",$J19&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E19,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E19,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J19"/>
+      <c r="J19" s="67" t="s">
+        <v>206</v>
+      </c>
       <c r="K19" s="68" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="O19" s="2" t="str">
         <f>'Definición técnica de imagenes'!A31</f>
         <v>F10</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="11" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" s="11" customFormat="1" ht="209.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="str">
         <f t="shared" si="6"/>
         <v>IMG11</v>
@@ -4193,9 +3998,7 @@
         <f ca="1">IF(OR($B20&lt;&gt;"",$J20&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E20,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E20,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J20" s="64" t="s">
-        <v>207</v>
-      </c>
+      <c r="J20" s="64"/>
       <c r="K20" s="66" t="s">
         <v>208</v>
       </c>
@@ -4204,7 +4007,7 @@
         <v>F10B</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="11" customFormat="1" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" s="11" customFormat="1" ht="214.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="str">
         <f t="shared" si="6"/>
         <v>IMG12</v>
@@ -4219,7 +4022,9 @@
       <c r="D21" s="63" t="s">
         <v>192</v>
       </c>
-      <c r="E21" s="63"/>
+      <c r="E21" s="63" t="s">
+        <v>153</v>
+      </c>
       <c r="F21" s="13" t="str">
         <f t="shared" si="4"/>
         <v>CN_10_11_CO_IMG12_small</v>
@@ -4236,31 +4041,33 @@
         <f ca="1">IF(OR($B21&lt;&gt;"",$J21&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E21,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E21,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J21"/>
+      <c r="J21" s="66"/>
       <c r="K21" s="66" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="O21" s="2" t="str">
         <f>'Definición técnica de imagenes'!A33</f>
         <v>F11</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="11" customFormat="1" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" s="11" customFormat="1" ht="169.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="str">
         <f t="shared" si="6"/>
         <v>IMG13</v>
       </c>
       <c r="B22" s="62" t="s">
-        <v>197</v>
+        <v>209</v>
       </c>
       <c r="C22" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D22" s="63" t="s">
-        <v>192</v>
-      </c>
-      <c r="E22" s="63"/>
+        <v>195</v>
+      </c>
+      <c r="E22" s="63" t="s">
+        <v>154</v>
+      </c>
       <c r="F22" s="13" t="str">
         <f t="shared" si="4"/>
         <v>CN_10_11_CO_IMG13_small</v>
@@ -4278,30 +4085,30 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J22" s="63"/>
-      <c r="K22" s="69" t="s">
-        <v>210</v>
-      </c>
+      <c r="K22" s="69"/>
       <c r="O22" s="2" t="str">
         <f>'Definición técnica de imagenes'!A34</f>
         <v>F12</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="11" customFormat="1" ht="195.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" s="11" customFormat="1" ht="178.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="str">
         <f t="shared" si="6"/>
         <v>IMG14</v>
       </c>
       <c r="B23" s="62" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="C23" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D23" s="63" t="s">
-        <v>192</v>
-      </c>
-      <c r="E23" s="63"/>
+        <v>195</v>
+      </c>
+      <c r="E23" s="63" t="s">
+        <v>154</v>
+      </c>
       <c r="F23" s="13" t="str">
         <f t="shared" si="4"/>
         <v>CN_10_11_CO_IMG14_small</v>
@@ -4319,15 +4126,13 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J23" s="64"/>
-      <c r="K23" s="64" t="s">
-        <v>209</v>
-      </c>
+      <c r="K23" s="64"/>
       <c r="O23" s="2" t="str">
         <f>'Definición técnica de imagenes'!A35</f>
         <v>F13</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="11" customFormat="1" ht="273" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" s="11" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="str">
         <f t="shared" si="6"/>
         <v>IMG15</v>
@@ -4370,7 +4175,7 @@
         <v>F13B</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="11" customFormat="1" ht="269.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" s="11" customFormat="1" ht="147" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="str">
         <f t="shared" si="6"/>
         <v>IMG16</v>
@@ -4405,162 +4210,134 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J25" s="63"/>
-      <c r="K25" s="65" t="s">
+      <c r="K25" s="64" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="26" spans="1:15" s="11" customFormat="1" ht="261.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="str">
         <f t="shared" si="6"/>
-        <v>IMG17</v>
-      </c>
-      <c r="B26" s="62" t="s">
-        <v>212</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B26" s="62"/>
       <c r="C26" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Cuaderno de Estudio</v>
-      </c>
-      <c r="D26" s="63" t="s">
-        <v>194</v>
-      </c>
-      <c r="E26" s="63" t="s">
-        <v>154</v>
-      </c>
+        <v/>
+      </c>
+      <c r="D26" s="63"/>
+      <c r="E26" s="63"/>
       <c r="F26" s="13" t="str">
         <f t="shared" si="4"/>
-        <v>CN_10_11_CO_IMG17_small</v>
+        <v/>
       </c>
       <c r="G26" s="13" t="str">
         <f ca="1">IF($F26&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E26,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>526 x 370 px</v>
+        <v/>
       </c>
       <c r="H26" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>CN_10_11_CO_IMG17_zoom</v>
+        <v/>
       </c>
       <c r="I26" s="13" t="str">
         <f ca="1">IF(OR($B26&lt;&gt;"",$J26&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E26,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E26,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 600 px</v>
+        <v/>
       </c>
       <c r="J26" s="63"/>
       <c r="K26" s="64"/>
     </row>
-    <row r="27" spans="1:15" s="11" customFormat="1" ht="236.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="str">
         <f t="shared" si="6"/>
-        <v>IMG18</v>
-      </c>
-      <c r="B27" s="62" t="s">
-        <v>213</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B27" s="62"/>
       <c r="C27" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Cuaderno de Estudio</v>
-      </c>
-      <c r="D27" s="63" t="s">
-        <v>194</v>
-      </c>
-      <c r="E27" s="63" t="s">
-        <v>154</v>
-      </c>
+        <v/>
+      </c>
+      <c r="D27" s="63"/>
+      <c r="E27" s="63"/>
       <c r="F27" s="13" t="str">
         <f t="shared" si="4"/>
-        <v>CN_10_11_CO_IMG18_small</v>
+        <v/>
       </c>
       <c r="G27" s="13" t="str">
         <f ca="1">IF($F27&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E27,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>526 x 370 px</v>
+        <v/>
       </c>
       <c r="H27" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>CN_10_11_CO_IMG18_zoom</v>
+        <v/>
       </c>
       <c r="I27" s="13" t="str">
         <f ca="1">IF(OR($B27&lt;&gt;"",$J27&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E27,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E27,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 600 px</v>
+        <v/>
       </c>
       <c r="J27" s="64"/>
       <c r="K27" s="64"/>
       <c r="O27" s="2"/>
     </row>
-    <row r="28" spans="1:15" s="11" customFormat="1" ht="234" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="str">
         <f t="shared" si="6"/>
-        <v>IMG19</v>
-      </c>
-      <c r="B28" s="62" t="s">
-        <v>197</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B28" s="62"/>
       <c r="C28" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Cuaderno de Estudio</v>
-      </c>
-      <c r="D28" s="63" t="s">
-        <v>192</v>
-      </c>
-      <c r="E28" s="63" t="s">
-        <v>153</v>
-      </c>
+        <v/>
+      </c>
+      <c r="D28" s="63"/>
+      <c r="E28" s="63"/>
       <c r="F28" s="13" t="str">
         <f t="shared" si="4"/>
-        <v>CN_10_11_CO_IMG19_small</v>
+        <v/>
       </c>
       <c r="G28" s="13" t="str">
         <f ca="1">IF($F28&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E28,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>526 x 370 px</v>
+        <v/>
       </c>
       <c r="H28" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>CN_10_11_CO_IMG19_zoom</v>
+        <v/>
       </c>
       <c r="I28" s="13" t="str">
         <f ca="1">IF(OR($B28&lt;&gt;"",$J28&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E28,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E28,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 600 px</v>
+        <v/>
       </c>
       <c r="J28" s="64"/>
-      <c r="K28" s="64" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" s="11" customFormat="1" ht="170.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K28" s="64"/>
+    </row>
+    <row r="29" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="str">
         <f t="shared" si="6"/>
-        <v>IMG20</v>
-      </c>
-      <c r="B29" s="62" t="s">
-        <v>197</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B29" s="62"/>
       <c r="C29" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Cuaderno de Estudio</v>
-      </c>
-      <c r="D29" s="63" t="s">
-        <v>192</v>
-      </c>
-      <c r="E29" s="63" t="s">
-        <v>153</v>
-      </c>
+        <v/>
+      </c>
+      <c r="D29" s="63"/>
+      <c r="E29" s="63"/>
       <c r="F29" s="13" t="str">
         <f t="shared" si="4"/>
-        <v>CN_10_11_CO_IMG20_small</v>
+        <v/>
       </c>
       <c r="G29" s="13" t="str">
         <f ca="1">IF($F29&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E29,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>526 x 370 px</v>
+        <v/>
       </c>
       <c r="H29" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>CN_10_11_CO_IMG20_zoom</v>
+        <v/>
       </c>
       <c r="I29" s="13" t="str">
         <f ca="1">IF(OR($B29&lt;&gt;"",$J29&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E29,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E29,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 600 px</v>
+        <v/>
       </c>
       <c r="J29" s="64"/>
-      <c r="K29" s="64" t="s">
-        <v>214</v>
-      </c>
+      <c r="K29" s="64"/>
     </row>
     <row r="30" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="str">
@@ -7061,127 +6838,77 @@
   <oleObjects>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="PBrush" shapeId="2052" r:id="rId4">
+        <oleObject progId="PBrush" shapeId="2051" r:id="rId4">
           <objectPr defaultSize="0" autoPict="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>9</xdr:col>
-                <xdr:colOff>1724025</xdr:colOff>
+                <xdr:colOff>685800</xdr:colOff>
                 <xdr:row>11</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:rowOff>38100</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>9</xdr:col>
-                <xdr:colOff>2676525</xdr:colOff>
+                <xdr:colOff>1638300</xdr:colOff>
                 <xdr:row>11</xdr:row>
-                <xdr:rowOff>2238375</xdr:rowOff>
+                <xdr:rowOff>1343025</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="PBrush" shapeId="2052" r:id="rId4"/>
+        <oleObject progId="PBrush" shapeId="2051" r:id="rId4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="PBrush" shapeId="2062" r:id="rId6">
+        <oleObject progId="PBrush" shapeId="2052" r:id="rId6">
           <objectPr defaultSize="0" autoPict="0" r:id="rId7">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>9</xdr:col>
-                <xdr:colOff>133350</xdr:colOff>
+                <xdr:colOff>219075</xdr:colOff>
                 <xdr:row>16</xdr:row>
-                <xdr:rowOff>228600</xdr:rowOff>
+                <xdr:rowOff>409575</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>9</xdr:col>
-                <xdr:colOff>3943350</xdr:colOff>
+                <xdr:colOff>4010025</xdr:colOff>
                 <xdr:row>16</xdr:row>
-                <xdr:rowOff>2562225</xdr:rowOff>
+                <xdr:rowOff>2705100</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="PBrush" shapeId="2062" r:id="rId6"/>
+        <oleObject progId="PBrush" shapeId="2052" r:id="rId6"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="PBrush" shapeId="2063" r:id="rId8">
+        <oleObject progId="PBrush" shapeId="2053" r:id="rId8">
           <objectPr defaultSize="0" autoPict="0" r:id="rId9">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>9</xdr:col>
                 <xdr:colOff>200025</xdr:colOff>
                 <xdr:row>17</xdr:row>
-                <xdr:rowOff>523875</xdr:rowOff>
+                <xdr:rowOff>57150</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>9</xdr:col>
                 <xdr:colOff>3876675</xdr:colOff>
                 <xdr:row>17</xdr:row>
-                <xdr:rowOff>2552700</xdr:rowOff>
+                <xdr:rowOff>2085975</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="PBrush" shapeId="2063" r:id="rId8"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <oleObject progId="PBrush" shapeId="2064" r:id="rId10">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId11">
-            <anchor moveWithCells="1" sizeWithCells="1">
-              <from>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>561975</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>276225</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>3771900</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>2343150</xdr:rowOff>
-              </to>
-            </anchor>
-          </objectPr>
-        </oleObject>
-      </mc:Choice>
-      <mc:Fallback>
-        <oleObject progId="PBrush" shapeId="2064" r:id="rId10"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <oleObject progId="PBrush" shapeId="2066" r:id="rId12">
-          <objectPr defaultSize="0" r:id="rId13">
-            <anchor moveWithCells="1" sizeWithCells="1">
-              <from>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>323850</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>390525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>2009775</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>1200150</xdr:rowOff>
-              </to>
-            </anchor>
-          </objectPr>
-        </oleObject>
-      </mc:Choice>
-      <mc:Fallback>
-        <oleObject progId="PBrush" shapeId="2066" r:id="rId12"/>
+        <oleObject progId="PBrush" shapeId="2053" r:id="rId8"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </oleObjects>

</xml_diff>